<commit_message>
Update texture index spreadsheet
</commit_message>
<xml_diff>
--- a/resource/textures/texture-index.xlsx
+++ b/resource/textures/texture-index.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="texture_index" localSheetId="0">Sheet1!$A$1:$B$1374</definedName>
+    <definedName name="texture_index" localSheetId="0">Sheet1!$A$1:$B$1404</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="1373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="1404">
   <si>
     <t>Brick Blue</t>
   </si>
@@ -4151,6 +4151,99 @@
   </si>
   <si>
     <t>qormas ground snow 2</t>
+  </si>
+  <si>
+    <t>qormas ice</t>
+  </si>
+  <si>
+    <t>jixa-rocks</t>
+  </si>
+  <si>
+    <t>jixa-grass</t>
+  </si>
+  <si>
+    <t>jixa-dirt-road</t>
+  </si>
+  <si>
+    <t>jixa-plank-side</t>
+  </si>
+  <si>
+    <t>jixa-plank-top</t>
+  </si>
+  <si>
+    <t>jixa-fountain-side</t>
+  </si>
+  <si>
+    <t>jixa-fountain-side2</t>
+  </si>
+  <si>
+    <t>jixa - fireplace</t>
+  </si>
+  <si>
+    <t>jixa-build-a-1</t>
+  </si>
+  <si>
+    <t>jixa : build 1 - roof (Thatch)</t>
+  </si>
+  <si>
+    <t>jixa-build-a-2 (door)</t>
+  </si>
+  <si>
+    <t>jixa-build-a-2</t>
+  </si>
+  <si>
+    <t>jixa-build-a-3</t>
+  </si>
+  <si>
+    <t>jixa: dragon transparen</t>
+  </si>
+  <si>
+    <t>jixa-build-b-1</t>
+  </si>
+  <si>
+    <t>jixa-build-b-2</t>
+  </si>
+  <si>
+    <t>jixa-build-b-3 (door)</t>
+  </si>
+  <si>
+    <t>jixa-build-b-4</t>
+  </si>
+  <si>
+    <t>jixa-build-b-5</t>
+  </si>
+  <si>
+    <t>jixa-build-b-5 (roof)</t>
+  </si>
+  <si>
+    <t>jixa-build-c-1</t>
+  </si>
+  <si>
+    <t>jixa-build-c-2</t>
+  </si>
+  <si>
+    <t>jixa-fance-2</t>
+  </si>
+  <si>
+    <t>jixa - fireplace - top</t>
+  </si>
+  <si>
+    <t>jixa - build d 1</t>
+  </si>
+  <si>
+    <t>jixa - build d 2 (roof)</t>
+  </si>
+  <si>
+    <t>jixa - build d 3 (door)</t>
+  </si>
+  <si>
+    <t>jala - ruin - pillar</t>
+  </si>
+  <si>
+    <t>jala - pillar-top</t>
+  </si>
+  <si>
+    <t>jala - fance</t>
   </si>
 </sst>
 </file>
@@ -4498,10 +4591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1390"/>
+  <dimension ref="A1:B1421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1369" workbookViewId="0">
-      <selection activeCell="B1391" sqref="B1391"/>
+    <sheetView tabSelected="1" topLeftCell="A1403" workbookViewId="0">
+      <selection activeCell="D1371" sqref="D1371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15224,410 +15317,658 @@
     </row>
     <row r="1340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1340" s="2">
-        <v>50002</v>
+        <v>20200</v>
       </c>
       <c r="B1340" s="1" t="s">
-        <v>1330</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1341" s="2">
-        <v>50003</v>
+        <v>20201</v>
       </c>
       <c r="B1341" s="1" t="s">
-        <v>1331</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1342" s="2">
-        <v>50004</v>
+        <v>20202</v>
       </c>
       <c r="B1342" s="1" t="s">
-        <v>1332</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1343" s="2">
-        <v>50005</v>
-      </c>
-      <c r="B1343" s="1" t="s">
-        <v>1333</v>
+        <v>20203</v>
+      </c>
+      <c r="B1343" t="s">
+        <v>1377</v>
       </c>
     </row>
     <row r="1344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1344" s="2">
-        <v>50050</v>
-      </c>
-      <c r="B1344" s="1" t="s">
-        <v>1334</v>
+        <v>20204</v>
+      </c>
+      <c r="B1344" t="s">
+        <v>1378</v>
       </c>
     </row>
     <row r="1345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1345" s="2">
-        <v>50051</v>
-      </c>
-      <c r="B1345" s="1" t="s">
-        <v>1335</v>
+        <v>20205</v>
+      </c>
+      <c r="B1345" t="s">
+        <v>1379</v>
       </c>
     </row>
     <row r="1346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1346" s="2">
-        <v>50052</v>
-      </c>
-      <c r="B1346" s="1" t="s">
-        <v>1336</v>
+        <v>20206</v>
+      </c>
+      <c r="B1346" t="s">
+        <v>1380</v>
       </c>
     </row>
     <row r="1347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1347" s="2">
-        <v>50053</v>
-      </c>
-      <c r="B1347" s="1" t="s">
-        <v>1337</v>
+        <v>20207</v>
+      </c>
+      <c r="B1347" t="s">
+        <v>1381</v>
       </c>
     </row>
     <row r="1348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1348" s="2">
-        <v>50054</v>
-      </c>
-      <c r="B1348" s="1" t="s">
-        <v>1338</v>
+        <v>20208</v>
+      </c>
+      <c r="B1348" t="s">
+        <v>1382</v>
       </c>
     </row>
     <row r="1349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1349" s="2">
-        <v>50055</v>
-      </c>
-      <c r="B1349" s="1" t="s">
-        <v>1338</v>
+        <v>20209</v>
+      </c>
+      <c r="B1349" t="s">
+        <v>1383</v>
       </c>
     </row>
     <row r="1350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1350" s="2">
-        <v>50056</v>
-      </c>
-      <c r="B1350" s="1" t="s">
-        <v>1338</v>
+        <v>20210</v>
+      </c>
+      <c r="B1350" t="s">
+        <v>1384</v>
       </c>
     </row>
     <row r="1351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1351" s="2">
-        <v>50057</v>
-      </c>
-      <c r="B1351" s="1" t="s">
-        <v>1339</v>
+        <v>20211</v>
+      </c>
+      <c r="B1351" t="s">
+        <v>1385</v>
       </c>
     </row>
     <row r="1352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1352" s="2">
-        <v>50058</v>
-      </c>
-      <c r="B1352" s="1" t="s">
-        <v>1340</v>
+        <v>20212</v>
+      </c>
+      <c r="B1352" t="s">
+        <v>1386</v>
       </c>
     </row>
     <row r="1353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1353" s="2">
-        <v>50059</v>
-      </c>
-      <c r="B1353" s="1" t="s">
-        <v>1340</v>
+        <v>20213</v>
+      </c>
+      <c r="B1353" t="s">
+        <v>1387</v>
       </c>
     </row>
     <row r="1354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1354" s="2">
-        <v>50060</v>
-      </c>
-      <c r="B1354" s="1" t="s">
-        <v>1340</v>
+        <v>20214</v>
+      </c>
+      <c r="B1354" t="s">
+        <v>1388</v>
       </c>
     </row>
     <row r="1355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1355" s="2">
-        <v>50061</v>
-      </c>
-      <c r="B1355" s="1" t="s">
-        <v>1341</v>
+        <v>20215</v>
+      </c>
+      <c r="B1355" t="s">
+        <v>1389</v>
       </c>
     </row>
     <row r="1356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1356" s="2">
-        <v>50062</v>
-      </c>
-      <c r="B1356" s="1" t="s">
-        <v>1342</v>
+        <v>20216</v>
+      </c>
+      <c r="B1356" t="s">
+        <v>1390</v>
       </c>
     </row>
     <row r="1357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1357" s="2">
-        <v>50063</v>
-      </c>
-      <c r="B1357" s="1" t="s">
-        <v>1343</v>
+        <v>20217</v>
+      </c>
+      <c r="B1357" t="s">
+        <v>1391</v>
       </c>
     </row>
     <row r="1358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1358" s="2">
-        <v>50064</v>
-      </c>
-      <c r="B1358" s="1" t="s">
-        <v>1344</v>
+        <v>20218</v>
+      </c>
+      <c r="B1358" t="s">
+        <v>1392</v>
       </c>
     </row>
     <row r="1359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1359" s="2">
-        <v>50065</v>
-      </c>
-      <c r="B1359" s="1" t="s">
-        <v>1345</v>
+        <v>20219</v>
+      </c>
+      <c r="B1359" t="s">
+        <v>1393</v>
       </c>
     </row>
     <row r="1360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1360" s="2">
-        <v>50066</v>
-      </c>
-      <c r="B1360" s="1" t="s">
-        <v>1346</v>
+        <v>20220</v>
+      </c>
+      <c r="B1360" t="s">
+        <v>1394</v>
       </c>
     </row>
     <row r="1361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1361" s="2">
-        <v>50067</v>
-      </c>
-      <c r="B1361" s="1" t="s">
-        <v>1346</v>
+        <v>20221</v>
+      </c>
+      <c r="B1361" t="s">
+        <v>1395</v>
       </c>
     </row>
     <row r="1362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1362" s="2">
-        <v>50068</v>
-      </c>
-      <c r="B1362" s="1" t="s">
-        <v>1346</v>
+        <v>20222</v>
+      </c>
+      <c r="B1362" t="s">
+        <v>1396</v>
       </c>
     </row>
     <row r="1363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1363" s="2">
-        <v>50069</v>
-      </c>
-      <c r="B1363" s="1" t="s">
-        <v>1347</v>
+        <v>20223</v>
+      </c>
+      <c r="B1363" t="s">
+        <v>1397</v>
       </c>
     </row>
     <row r="1364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1364" s="2">
-        <v>50070</v>
-      </c>
-      <c r="B1364" s="1" t="s">
-        <v>1348</v>
+        <v>20224</v>
+      </c>
+      <c r="B1364" t="s">
+        <v>1398</v>
       </c>
     </row>
     <row r="1365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1365" s="2">
-        <v>50071</v>
-      </c>
-      <c r="B1365" s="1" t="s">
-        <v>1348</v>
+        <v>20225</v>
+      </c>
+      <c r="B1365" t="s">
+        <v>1399</v>
       </c>
     </row>
     <row r="1366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1366" s="2">
-        <v>50072</v>
-      </c>
-      <c r="B1366" s="1" t="s">
-        <v>1348</v>
+        <v>20226</v>
+      </c>
+      <c r="B1366" t="s">
+        <v>1400</v>
       </c>
     </row>
     <row r="1367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1367" s="2">
-        <v>50073</v>
-      </c>
-      <c r="B1367" s="1" t="s">
-        <v>1349</v>
+        <v>20227</v>
+      </c>
+      <c r="B1367" t="s">
+        <v>1401</v>
       </c>
     </row>
     <row r="1368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1368" s="2">
-        <v>50074</v>
-      </c>
-      <c r="B1368" s="1" t="s">
-        <v>1350</v>
+        <v>20228</v>
+      </c>
+      <c r="B1368" t="s">
+        <v>1402</v>
       </c>
     </row>
     <row r="1369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1369" s="2">
-        <v>50075</v>
-      </c>
-      <c r="B1369" s="1" t="s">
-        <v>1351</v>
+        <v>20229</v>
+      </c>
+      <c r="B1369" t="s">
+        <v>1403</v>
       </c>
     </row>
     <row r="1370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1370" s="2">
-        <v>50076</v>
+        <v>50002</v>
       </c>
       <c r="B1370" s="1" t="s">
-        <v>1352</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="1371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1371" s="2">
-        <v>50077</v>
+        <v>50003</v>
       </c>
       <c r="B1371" s="1" t="s">
-        <v>1353</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1372" s="2">
-        <v>60001</v>
+        <v>50004</v>
       </c>
       <c r="B1372" s="1" t="s">
-        <v>1354</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1373" s="2">
-        <v>60002</v>
+        <v>50005</v>
       </c>
       <c r="B1373" s="1" t="s">
-        <v>1355</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="1374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1374" s="2">
-        <v>60003</v>
+        <v>50050</v>
       </c>
       <c r="B1374" s="1" t="s">
-        <v>1356</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1375" s="2">
-        <v>61001</v>
+        <v>50051</v>
       </c>
       <c r="B1375" s="1" t="s">
-        <v>1357</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1376" s="2">
-        <v>61002</v>
+        <v>50052</v>
       </c>
       <c r="B1376" s="1" t="s">
-        <v>1358</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1377" s="2">
-        <v>61003</v>
+        <v>50053</v>
       </c>
       <c r="B1377" s="1" t="s">
-        <v>1359</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1378" s="2">
-        <v>61004</v>
+        <v>50054</v>
       </c>
       <c r="B1378" s="1" t="s">
-        <v>1360</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1379" s="2">
-        <v>61005</v>
+        <v>50055</v>
       </c>
       <c r="B1379" s="1" t="s">
-        <v>1361</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1380" s="2">
-        <v>61006</v>
+        <v>50056</v>
       </c>
       <c r="B1380" s="1" t="s">
-        <v>1362</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1381" s="2">
-        <v>61007</v>
+        <v>50057</v>
       </c>
       <c r="B1381" s="1" t="s">
-        <v>1363</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="1382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1382" s="2">
-        <v>61008</v>
+        <v>50058</v>
       </c>
       <c r="B1382" s="1" t="s">
-        <v>1364</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1383" s="2">
-        <v>61009</v>
+        <v>50059</v>
       </c>
       <c r="B1383" s="1" t="s">
-        <v>1365</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1384" s="2">
-        <v>61010</v>
+        <v>50060</v>
       </c>
       <c r="B1384" s="1" t="s">
-        <v>1366</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1385" s="2">
-        <v>61011</v>
+        <v>50061</v>
       </c>
       <c r="B1385" s="1" t="s">
-        <v>1367</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1386" s="2">
-        <v>61012</v>
+        <v>50062</v>
       </c>
       <c r="B1386" s="1" t="s">
-        <v>1368</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1387" s="2">
-        <v>61013</v>
+        <v>50063</v>
       </c>
       <c r="B1387" s="1" t="s">
-        <v>1369</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1388" s="2">
-        <v>61014</v>
+        <v>50064</v>
       </c>
       <c r="B1388" s="1" t="s">
-        <v>1370</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1389" s="2">
-        <v>61015</v>
-      </c>
-      <c r="B1389" t="s">
-        <v>1371</v>
+        <v>50065</v>
+      </c>
+      <c r="B1389" s="1" t="s">
+        <v>1345</v>
       </c>
     </row>
     <row r="1390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1390" s="2">
+        <v>50066</v>
+      </c>
+      <c r="B1390" s="1" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1391" s="2">
+        <v>50067</v>
+      </c>
+      <c r="B1391" s="1" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1392" s="2">
+        <v>50068</v>
+      </c>
+      <c r="B1392" s="1" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1393" s="2">
+        <v>50069</v>
+      </c>
+      <c r="B1393" s="1" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1394" s="2">
+        <v>50070</v>
+      </c>
+      <c r="B1394" s="1" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1395" s="2">
+        <v>50071</v>
+      </c>
+      <c r="B1395" s="1" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1396" s="2">
+        <v>50072</v>
+      </c>
+      <c r="B1396" s="1" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1397" s="2">
+        <v>50073</v>
+      </c>
+      <c r="B1397" s="1" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1398" s="2">
+        <v>50074</v>
+      </c>
+      <c r="B1398" s="1" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1399" s="2">
+        <v>50075</v>
+      </c>
+      <c r="B1399" s="1" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1400" s="2">
+        <v>50076</v>
+      </c>
+      <c r="B1400" s="1" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1401" s="2">
+        <v>50077</v>
+      </c>
+      <c r="B1401" s="1" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1402" s="2">
+        <v>60001</v>
+      </c>
+      <c r="B1402" s="1" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1403" s="2">
+        <v>60002</v>
+      </c>
+      <c r="B1403" s="1" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1404" s="2">
+        <v>60003</v>
+      </c>
+      <c r="B1404" s="1" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1405" s="2">
+        <v>61001</v>
+      </c>
+      <c r="B1405" s="1" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1406" s="2">
+        <v>61002</v>
+      </c>
+      <c r="B1406" s="1" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1407" s="2">
+        <v>61003</v>
+      </c>
+      <c r="B1407" s="1" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1408" s="2">
+        <v>61004</v>
+      </c>
+      <c r="B1408" s="1" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1409" s="2">
+        <v>61005</v>
+      </c>
+      <c r="B1409" s="1" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1410" s="2">
+        <v>61006</v>
+      </c>
+      <c r="B1410" s="1" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1411" s="2">
+        <v>61007</v>
+      </c>
+      <c r="B1411" s="1" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1412" s="2">
+        <v>61008</v>
+      </c>
+      <c r="B1412" s="1" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1413" s="2">
+        <v>61009</v>
+      </c>
+      <c r="B1413" s="1" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1414" s="2">
+        <v>61010</v>
+      </c>
+      <c r="B1414" s="1" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1415" s="2">
+        <v>61011</v>
+      </c>
+      <c r="B1415" s="1" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1416" s="2">
+        <v>61012</v>
+      </c>
+      <c r="B1416" s="1" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1417" s="2">
+        <v>61013</v>
+      </c>
+      <c r="B1417" s="1" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1418" s="2">
+        <v>61014</v>
+      </c>
+      <c r="B1418" s="1" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1419" s="2">
+        <v>61015</v>
+      </c>
+      <c r="B1419" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1420" s="2">
         <v>61016</v>
       </c>
-      <c r="B1390" s="1" t="s">
+      <c r="B1420" s="1" t="s">
         <v>1372</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1421" s="2">
+        <v>61017</v>
+      </c>
+      <c r="B1421" s="1" t="s">
+        <v>1373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>